<commit_message>
resrc: update tbk related models, styles and scripts
Updated TBk QField Themes, a few TBK related graphical modeller workflows and some related styles.
</commit_message>
<xml_diff>
--- a/auxiliary_ressources/TBk_QField_Themes.xlsx
+++ b/auxiliary_ressources/TBk_QField_Themes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\bfh.ch\data\HAFL\7 WWI\74a FF WG\742a Aktuell\L.012359-52-WFOM_TBk_II\01_TBk\Dev\QGIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbh1\Projects\H07_TBk\Dev\TBk_QGIS_Plugin\auxiliary_ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408DFE62-52A3-4722-92D1-45601F80C8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC9A2B9-3D39-4836-B74E-D89EC36C12FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12165" yWindow="-21720" windowWidth="51840" windowHeight="21390" xr2:uid="{A9DD7484-4502-4BD0-85F4-5E5138CE816F}"/>
+    <workbookView xWindow="8100" yWindow="-16545" windowWidth="22935" windowHeight="15045" xr2:uid="{A9DD7484-4502-4BD0-85F4-5E5138CE816F}"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="4" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
   <si>
     <t>11 TBk hdom Oberschicht (yyyy)</t>
   </si>
@@ -365,9 +365,6 @@
     <t>Oberschicht Veränderungen (hdom&gt;30m) [OS VÄ]</t>
   </si>
   <si>
-    <t>42_20xx-20yy TBk Oberschicht Veränderungen (hdom&gt;30m) [OS VÄ]</t>
-  </si>
-  <si>
     <t>OS Veränderung (alle)</t>
   </si>
   <si>
@@ -393,6 +390,12 @@
   </si>
   <si>
     <t>Name DE</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>2b</t>
   </si>
 </sst>
 </file>
@@ -907,7 +910,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -917,7 +920,7 @@
     <col min="4" max="4" width="7.5703125" style="6" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" style="10" customWidth="1"/>
     <col min="8" max="8" width="30.85546875" style="15" customWidth="1"/>
     <col min="9" max="9" width="3.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -955,7 +958,7 @@
         <v>40</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>49</v>
@@ -1137,17 +1140,17 @@
         <v>6</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="G8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>16_Dendro Vorrat m³</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1417,7 +1420,7 @@
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1488,30 +1491,24 @@
       <c r="B22" s="7">
         <v>4</v>
       </c>
-      <c r="C22" s="8">
-        <v>2</v>
+      <c r="C22" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>42_20xx-20yy TBk Oberschicht Veränderungen (hdom&gt;30m) [OS VÄ]</v>
+        <f>_xlfn.CONCAT(B22,C22,"_",IF(D22="","",_xlfn.CONCAT(D22," ")),IF(F22="","",_xlfn.CONCAT(F22," ")),E22)</f>
+        <v>42a_20xx-20yy TBk OS Veränderung (alle)</v>
       </c>
       <c r="H22" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1521,23 +1518,30 @@
       <c r="B23" s="7">
         <v>4</v>
       </c>
-      <c r="C23" s="8">
-        <v>2</v>
+      <c r="C23" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>95</v>
+      <c r="G23" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>42b_20xx-20yy TBk Oberschicht Veränderungen (hdom&gt;30m) [OS VÄ]</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1554,7 +1558,7 @@
         <v>41</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G24" s="10" t="str">
         <f t="shared" si="1"/>

</xml_diff>